<commit_message>
Added outputs and experimentations for DS2 DT
</commit_message>
<xml_diff>
--- a/Data set release 1/ds1/ds1_stats.xlsx
+++ b/Data set release 1/ds1/ds1_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realn\OneDrive\Documents\git\soen472_mp2\Data set release 1\ds1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4105CBCF-C4AC-4B82-A628-029BDCD9555E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE95091-258E-4901-BF9B-0270588A20C9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4020" activeTab="3" xr2:uid="{E3F65C83-32B3-4C7A-966E-A0762FD703F3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4020" activeTab="2" xr2:uid="{E3F65C83-32B3-4C7A-966E-A0762FD703F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
@@ -751,7 +751,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="E7" sqref="E1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -890,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7A6426-F1A3-479C-A068-38DE87B162FB}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1185,7 +1185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BB33D6-6C10-4352-926A-B786B339F69C}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added experimentations for DS1 NN
</commit_message>
<xml_diff>
--- a/Data set release 1/ds1/ds1_stats.xlsx
+++ b/Data set release 1/ds1/ds1_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realn\OneDrive\Documents\git\soen472_mp2\Data set release 1\ds1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE95091-258E-4901-BF9B-0270588A20C9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CF3824-DCFC-477D-8A54-27B4210E4A67}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4020" activeTab="2" xr2:uid="{E3F65C83-32B3-4C7A-966E-A0762FD703F3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
   <si>
     <t>Algorithm</t>
   </si>
@@ -205,6 +205,33 @@
   </si>
   <si>
     <t>Unpruned = true; minNumObj = 3</t>
+  </si>
+  <si>
+    <t>Different metrics</t>
+  </si>
+  <si>
+    <t>Should be somewhere between nb of classes and nb of attributes. More = better, but significantly slower</t>
+  </si>
+  <si>
+    <t>More epochs = reduced error, but longer run time</t>
+  </si>
+  <si>
+    <t>Can only be set if GUI not displayed</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Better metrics, up to a certain threshold</t>
+  </si>
+  <si>
+    <t>Better metrics</t>
+  </si>
+  <si>
+    <t>Worse metrics</t>
+  </si>
+  <si>
+    <t>Better at 0.2</t>
   </si>
 </sst>
 </file>
@@ -276,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -289,6 +316,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -890,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7A6426-F1A3-479C-A068-38DE87B162FB}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1109,65 +1139,131 @@
       <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>34</v>
       </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28">
+        <v>500</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>38</v>
       </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>39</v>
+      </c>
+      <c r="D30">
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>